<commit_message>
Validated to extract but not reformat docstring (end of day 8/3/23)
</commit_message>
<xml_diff>
--- a/tests/df_plan.xlsx
+++ b/tests/df_plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>routine_name</t>
   </si>
@@ -22,10 +22,13 @@
     <t>type</t>
   </si>
   <si>
-    <t>line_num_start</t>
+    <t>idx_start</t>
   </si>
   <si>
     <t>arguments</t>
+  </si>
+  <si>
+    <t>docstring</t>
   </si>
   <si>
     <t>ExampleProcedure</t>
@@ -56,6 +59,25 @@
 i|Integer|ByRef,
 j|Integer|ByRef,
 arg2|Variant|ByRef</t>
+  </si>
+  <si>
+    <t>' A docstring for a procedure 
+' 
+' JDL 12/13/21   Modified: 8/1/23 JDL 
+'</t>
+  </si>
+  <si>
+    <t>' Method1 docstring is 
+' multiline 
+' 
+' JDL 8/1/23 
+'</t>
+  </si>
+  <si>
+    <t>' Method2 docstring 
+' 
+' JDL 8/1/23 
+'</t>
   </si>
 </sst>
 </file>
@@ -413,13 +435,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,47 +454,59 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
       <c r="C4">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Validated df_plan with args, docstrings and vars_internal columns
</commit_message>
<xml_diff>
--- a/tests/df_plan.xlsx
+++ b/tests/df_plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>routine_name</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>docstring</t>
+  </si>
+  <si>
+    <t>vars_internal</t>
   </si>
   <si>
     <t>ExampleProcedure</t>
@@ -61,23 +64,26 @@
 arg2|Variant|ByRef</t>
   </si>
   <si>
-    <t>' A docstring for a procedure 
-' 
-' JDL 12/13/21   Modified: 8/1/23 JDL 
-'</t>
-  </si>
-  <si>
-    <t>' Method1 docstring is 
-' multiline 
-' 
-' JDL 8/1/23 
-'</t>
-  </si>
-  <si>
-    <t>' Method2 docstring 
-' 
-' JDL 8/1/23 
-'</t>
+    <t>A docstring for a procedure</t>
+  </si>
+  <si>
+    <t>Method1 docstring is
+multiline</t>
+  </si>
+  <si>
+    <t>Method2 docstring</t>
+  </si>
+  <si>
+    <t>i|Integer,
+j|Integer</t>
+  </si>
+  <si>
+    <t>cht|Chart|New,
+tbl|tblRowsCols|New</t>
+  </si>
+  <si>
+    <t>rng|Variant,
+tbl|Object</t>
   </si>
 </sst>
 </file>
@@ -435,13 +441,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,56 +463,68 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>